<commit_message>
First half of the ReadMe
</commit_message>
<xml_diff>
--- a/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
+++ b/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richter122\git-projects\openehr_flat_loader\Manual Tasks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Mapping CSV2openEHR" sheetId="1" r:id="rId1"/>
     <sheet name="FLAT_Paths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
   <si>
     <t>CSV-Column</t>
   </si>
@@ -362,8 +367,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,15 +401,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -446,7 +459,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -478,9 +491,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,6 +526,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -687,19 +702,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="130.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -721,611 +738,678 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
-      <formula1>FLAT_Paths!$A$2:$A$25</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
The mapping holds one Index Column for every index field in the path with the most index fields. The builder subsitutes the <<index>> occassions with the correct index number from the 1., 2., 3. and so on index column.
</commit_message>
<xml_diff>
--- a/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
+++ b/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
@@ -20,15 +20,291 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="114">
+  <si>
+    <t>FLAT-Path</t>
+  </si>
+  <si>
+    <t>bericht/category|code</t>
+  </si>
+  <si>
+    <t>bericht/context/bericht_id</t>
+  </si>
+  <si>
+    <t>bericht/context/status</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/pr_fix</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/art_des_pr_fix</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/vorsatzwort</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/vorname</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/familienname</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/nachname</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/geburtsname</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/namenszusatz</t>
+  </si>
+  <si>
+    <t>bericht/context/daten_zur_geburt&lt;&lt;index&gt;&gt;/geburtsdatum</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_todesangaben&lt;&lt;index&gt;&gt;/letzter_lebendzeitpunkt</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_todesangaben&lt;&lt;index&gt;&gt;/patient_verstorben</t>
+  </si>
+  <si>
+    <t>bericht/context/data_origin/organisationseinheit_name|code</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_geschlecht&lt;&lt;index&gt;&gt;/administratives_geschlecht|code</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/stra_e</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/postleitzahl</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/wohnort</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/land</t>
+  </si>
+  <si>
+    <t>bericht/context/start_time</t>
+  </si>
+  <si>
+    <t>bericht/context/setting|code</t>
+  </si>
+  <si>
+    <t>bericht/context/setting|value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungstyp</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/text_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/coded_text_value|code</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/coded_text_value|value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/multimedia_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/parsable_value|value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/parsable_value|formalism</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/state_value|code</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/state_value|value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/boolean_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|id</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|type</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|issuer</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|assigner</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/uri_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/ehr_uri_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|year</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|month</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|day</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|week</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|hour</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|minute</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|second</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/quantity_value|magnitude</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/quantity_value|unit</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/count_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/proportion_value|numerator</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/proportion_value|denominator</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/date_time_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/time_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/ordinal_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/date_value</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|name</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/language|code</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/language|terminology</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/encoding|code</t>
+  </si>
+  <si>
+    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/encoding|terminology</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/pseudonym</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|name</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/language|code</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/language|terminology</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/encoding|code</t>
+  </si>
+  <si>
+    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/encoding|terminology</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/alter_jahresanteil</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/alter_tagesanteil</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/berechnungsdatum</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/time</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|name</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/language|code</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/language|terminology</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/encoding|code</t>
+  </si>
+  <si>
+    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/encoding|terminology</t>
+  </si>
+  <si>
+    <t>bericht/composer|id</t>
+  </si>
+  <si>
+    <t>bericht/composer|id_scheme</t>
+  </si>
+  <si>
+    <t>bericht/composer|id_namespace</t>
+  </si>
+  <si>
+    <t>bericht/composer|name</t>
+  </si>
+  <si>
+    <t>bericht/language|code</t>
+  </si>
+  <si>
+    <t>bericht/language|terminology</t>
+  </si>
+  <si>
+    <t>bericht/territory|code</t>
+  </si>
+  <si>
+    <t>bericht/territory|terminology</t>
+  </si>
   <si>
     <t>CSV-Column</t>
   </si>
   <si>
-    <t>FLAT-Path</t>
-  </si>
-  <si>
-    <t>Index</t>
+    <t>1. Index</t>
   </si>
   <si>
     <t>Hinweis:</t>
@@ -86,282 +362,6 @@
   </si>
   <si>
     <t>bericht_composer</t>
-  </si>
-  <si>
-    <t>bericht/category|code</t>
-  </si>
-  <si>
-    <t>bericht/context/bericht_id</t>
-  </si>
-  <si>
-    <t>bericht/context/status</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/pr_fix</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/art_des_pr_fix</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/vorsatzwort</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/vorname</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/familienname</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/nachname</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/geburtsname</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/namenszusatz</t>
-  </si>
-  <si>
-    <t>bericht/context/daten_zur_geburt&lt;&lt;index&gt;&gt;/geburtsdatum</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_todesangaben&lt;&lt;index&gt;&gt;/letzter_lebendzeitpunkt</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_todesangaben&lt;&lt;index&gt;&gt;/patient_verstorben</t>
-  </si>
-  <si>
-    <t>bericht/context/data_origin/organisationseinheit_name|code</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_geschlecht&lt;&lt;index&gt;&gt;/administratives_geschlecht|code</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/stra_e</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/postleitzahl</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/wohnort</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/land</t>
-  </si>
-  <si>
-    <t>bericht/context/start_time</t>
-  </si>
-  <si>
-    <t>bericht/context/setting|code</t>
-  </si>
-  <si>
-    <t>bericht/context/setting|value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungstyp</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/text_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/coded_text_value|code</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/coded_text_value|value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/multimedia_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/parsable_value|value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/parsable_value|formalism</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/state_value|code</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/state_value|value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/boolean_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|id</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|type</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|issuer</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/identifier_value|assigner</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/uri_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/ehr_uri_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|year</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|month</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|day</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|week</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|hour</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|minute</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/duration_value|second</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/quantity_value|magnitude</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/quantity_value|unit</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/count_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/proportion_value|numerator</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/proportion_value|denominator</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/date_time_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/time_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/ordinal_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/versicherungsnummer/date_value</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/subject|name</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/language|code</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/language|terminology</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/encoding|code</t>
-  </si>
-  <si>
-    <t>bericht/versicherungsinformationen&lt;&lt;index&gt;&gt;/encoding|terminology</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/pseudonym</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/subject|name</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/language|code</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/language|terminology</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/encoding|code</t>
-  </si>
-  <si>
-    <t>bericht/umg_pseudonym&lt;&lt;index&gt;&gt;/encoding|terminology</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/alter_jahresanteil</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/alter_tagesanteil</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/berechnungsdatum</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/time</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id_scheme</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|id_namespace</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/subject|name</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/language|code</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/language|terminology</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/encoding|code</t>
-  </si>
-  <si>
-    <t>bericht/altersangaben&lt;&lt;index&gt;&gt;/encoding|terminology</t>
-  </si>
-  <si>
-    <t>bericht/composer|id</t>
-  </si>
-  <si>
-    <t>bericht/composer|id_scheme</t>
-  </si>
-  <si>
-    <t>bericht/composer|id_namespace</t>
-  </si>
-  <si>
-    <t>bericht/composer|name</t>
-  </si>
-  <si>
-    <t>bericht/language|code</t>
-  </si>
-  <si>
-    <t>bericht/language|terminology</t>
-  </si>
-  <si>
-    <t>bericht/territory|code</t>
-  </si>
-  <si>
-    <t>bericht/territory|terminology</t>
   </si>
 </sst>
 </file>
@@ -706,129 +706,123 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
-    <col min="4" max="4" width="130.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -838,97 +832,97 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$25</xm:f>
+            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
           </x14:formula1>
           <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
@@ -951,467 +945,467 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Upload of OPT in correct UTF-8 encoding and added some error handling
</commit_message>
<xml_diff>
--- a/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
+++ b/Manual Tasks/UMG_Stammdaten_MAPPING.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richter122\git-projects\openehr_flat_loader\Manual Tasks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="Mapping CSV2openEHR" sheetId="1" r:id="rId1"/>
     <sheet name="FLAT_Paths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>FLAT-Path</t>
   </si>
@@ -34,10 +29,10 @@
     <t>bericht/context/status</t>
   </si>
   <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/pr_fix</t>
-  </si>
-  <si>
-    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/art_des_pr_fix</t>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/präfix</t>
+  </si>
+  <si>
+    <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/art_des_präfix</t>
   </si>
   <si>
     <t>bericht/context/umg_personenname&lt;&lt;index&gt;&gt;/name_strukturiert/vorsatzwort</t>
@@ -73,7 +68,7 @@
     <t>bericht/context/umg_geschlecht&lt;&lt;index&gt;&gt;/administratives_geschlecht|code</t>
   </si>
   <si>
-    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/stra_e</t>
+    <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/straße</t>
   </si>
   <si>
     <t>bericht/context/umg_adresse&lt;&lt;index&gt;&gt;/postleitzahl</t>
@@ -367,8 +362,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,23 +396,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -459,7 +446,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,10 +478,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -526,7 +512,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -702,21 +687,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -730,7 +713,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -738,7 +721,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -746,664 +729,603 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>101</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>104</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+      <formula1>FLAT_Paths!$A$2:$A$93</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$93</xm:f>
-          </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A93"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1">
       <c r="A88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1">
       <c r="A91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1">
       <c r="A92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1">
       <c r="A93" t="s">
         <v>92</v>
       </c>

</xml_diff>